<commit_message>
add more data to xgboost model 2 years
</commit_message>
<xml_diff>
--- a/back_testing/datos/calendars/meta_11mar2025.xlsx
+++ b/back_testing/datos/calendars/meta_11mar2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bravi\projects\trade_python\back_testing\datos\calendars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B0DED9-9188-4FC5-829C-D489A5F1B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842610E7-E6AA-4D16-87F0-B4A642823F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{03A8C185-72E1-494D-A93C-6E08DDA5E9B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
   <si>
     <t>Morgan Stanley Technology, Media &amp; Telecom Conference</t>
   </si>
@@ -87,13 +87,391 @@
   </si>
   <si>
     <t>GTC AI Conference</t>
+  </si>
+  <si>
+    <t>Q3 2023 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q3 2023 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q2 2023 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q2 2023 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q1 2023 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q1 2023 Earnings Release</t>
+  </si>
+  <si>
+    <t>FY 2022 Earnings Call</t>
+  </si>
+  <si>
+    <t>FY 2022 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q3 2022 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q3 2022 Earnings Release</t>
+  </si>
+  <si>
+    <t>Interim 2022 Earnings Call</t>
+  </si>
+  <si>
+    <t>Interim 2022 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q1 2022 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q1 2022 Earnings Release</t>
+  </si>
+  <si>
+    <t>Morgan Stanley Technology, Media and Telecom Conference</t>
+  </si>
+  <si>
+    <t>FY 2021 Earnings Call</t>
+  </si>
+  <si>
+    <t>FY 2021 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q3 2021 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q3 2021 Earnings Release</t>
+  </si>
+  <si>
+    <t>Interim 2021 Earnings Call</t>
+  </si>
+  <si>
+    <t>Interim 2021 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q1 2021 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q1 2021 Earnings Release</t>
+  </si>
+  <si>
+    <t>GPU Technology Conference</t>
+  </si>
+  <si>
+    <t>FY 2020 Earnings Call</t>
+  </si>
+  <si>
+    <t>FY 2020 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q3 2020 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q3 2020 Earnings Release</t>
+  </si>
+  <si>
+    <t>6G Symposium</t>
+  </si>
+  <si>
+    <t>BigCommerce Make it Big Conference</t>
+  </si>
+  <si>
+    <t>Interim 2020 Earnings Call</t>
+  </si>
+  <si>
+    <t>Interim 2020 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q1 2020 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q1 2020 Earnings Release</t>
+  </si>
+  <si>
+    <t>FY 2019 Earnings Call</t>
+  </si>
+  <si>
+    <t>FY 2019 Earnings Release</t>
+  </si>
+  <si>
+    <t>Telecom Infra Project Summit</t>
+  </si>
+  <si>
+    <t>MarketplaceLIVE Conference</t>
+  </si>
+  <si>
+    <t>Q3 2019 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q3 2019 Earnings Release</t>
+  </si>
+  <si>
+    <t>Linley Fall Processor Conference</t>
+  </si>
+  <si>
+    <t>Arm Tech Conference</t>
+  </si>
+  <si>
+    <t>IBC Conference</t>
+  </si>
+  <si>
+    <t>Interim 2019 Earnings Call</t>
+  </si>
+  <si>
+    <t>Interim 2019 Earnings Release</t>
+  </si>
+  <si>
+    <t>Media, Entertainment and Technology Alliance Conference</t>
+  </si>
+  <si>
+    <t>AI Summit</t>
+  </si>
+  <si>
+    <t>Lightspeed Connect Conference</t>
+  </si>
+  <si>
+    <t>Inventures Conference</t>
+  </si>
+  <si>
+    <t>QTS Richmond Network Access Point Summit</t>
+  </si>
+  <si>
+    <t>Q1 2019 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q1 2019 Earnings Release</t>
+  </si>
+  <si>
+    <t>eTail Asia Conference</t>
+  </si>
+  <si>
+    <t>Brainstorm Design Conference</t>
+  </si>
+  <si>
+    <t>Morgan Stanley TMT Conference</t>
+  </si>
+  <si>
+    <t>MariaDB User Conference</t>
+  </si>
+  <si>
+    <t>FY 2018 Earnings Call</t>
+  </si>
+  <si>
+    <t>FY 2018 Earnings Release</t>
+  </si>
+  <si>
+    <t>IRPA AI Automation Innovation Conference</t>
+  </si>
+  <si>
+    <t>Q3 2018 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q3 2018 Earnings Release</t>
+  </si>
+  <si>
+    <t>HR Shared Services and Outsourcing Summit</t>
+  </si>
+  <si>
+    <t>NVIDIA GPU Technology Conference</t>
+  </si>
+  <si>
+    <t>Interim 2018 Earnings Call</t>
+  </si>
+  <si>
+    <t>Interim 2018 Earnings Release</t>
+  </si>
+  <si>
+    <t>Money20/20 Europe Conference</t>
+  </si>
+  <si>
+    <t>Q1 2018 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q1 2018 Earnings Release</t>
+  </si>
+  <si>
+    <t>FY 2017 Earnings Call</t>
+  </si>
+  <si>
+    <t>FY 2017 Earnings Release</t>
+  </si>
+  <si>
+    <t>Wells Fargo Event Information &amp; Logistics Tech Summit</t>
+  </si>
+  <si>
+    <t>Q3 2017 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q3 2017 Earnings Release</t>
+  </si>
+  <si>
+    <t>Interim 2017 Earnings Call</t>
+  </si>
+  <si>
+    <t>Interim 2017 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q1 2017 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q1 2017 Earnings Release</t>
+  </si>
+  <si>
+    <t>FY 2016 Earnings Call</t>
+  </si>
+  <si>
+    <t>FY 2016 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q3 2016 Earnings Call</t>
+  </si>
+  <si>
+    <t>Q3 2016 Earnings Release</t>
+  </si>
+  <si>
+    <t>Money20/20 Conference</t>
+  </si>
+  <si>
+    <t>Interim 2016 Earnings Call</t>
+  </si>
+  <si>
+    <t>Interim 2016 Earnings Release</t>
+  </si>
+  <si>
+    <t>Q1 2016 Earnings Call</t>
+  </si>
+  <si>
+    <t>Jefferies Media &amp; Communications Conference - Panel</t>
+  </si>
+  <si>
+    <t>Goldman Sachs Technology and Internet Conference</t>
+  </si>
+  <si>
+    <t>FY 2015 Earnings Call</t>
+  </si>
+  <si>
+    <t>UBS Global Media and Communications Conference</t>
+  </si>
+  <si>
+    <t>Q3 2015 Earnings Call</t>
+  </si>
+  <si>
+    <t>Money20/20 Conference - Keynote: Deborah Liu</t>
+  </si>
+  <si>
+    <t>Money20/20 Conference - Panel-Social Commerce: The Rise of the Buy Button</t>
+  </si>
+  <si>
+    <t>Interim 2015 Earnings Call</t>
+  </si>
+  <si>
+    <t>JPMorgan Global Technology, Media and Telecom Conference</t>
+  </si>
+  <si>
+    <t>Q1 2015 Earnings Call</t>
+  </si>
+  <si>
+    <t>Morgan Stanley Technology Media &amp; Telecom Conference</t>
+  </si>
+  <si>
+    <t>Goldman Sachs Technology &amp; Internet Conference</t>
+  </si>
+  <si>
+    <t>FY 2014 Earnings Call</t>
+  </si>
+  <si>
+    <r>
+      <t>Q1 2016 Earnings Release </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1D73DD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>After hours</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FY 2015 Earnings Release </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1D73DD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>After hours</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Q3 2015 Earnings Release </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1D73DD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>After hours</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Interim 2015 Earnings Release </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1D73DD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>After hours</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Q1 2015 Earnings Release </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1D73DD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>After hours</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FY 2014 Earnings Release </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1D73DD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>After hours</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +490,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF262626"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D73DD"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -497,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72095DC-1117-4747-8706-0F1D3C0C57FA}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -677,6 +1061,1502 @@
         <v>14</v>
       </c>
     </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2">
+        <v>45224.708333333336</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2">
+        <v>45224.677777777775</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2">
+        <v>45133.708333333336</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="2">
+        <v>45133.670138888891</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2">
+        <v>45077.541666666664</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2">
+        <v>45042.708333333336</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2">
+        <v>45042.67291666667</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2">
+        <v>44994.597222222219</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2">
+        <v>44958.708333333336</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="2">
+        <v>44958.670138888891</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="2">
+        <v>44860.708333333336</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="2">
+        <v>44860.670138888891</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2">
+        <v>44769.708333333336</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="2">
+        <v>44769.670138888891</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2">
+        <v>44706.541666666664</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2">
+        <v>44678.708333333336</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2">
+        <v>44678.670138888891</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2">
+        <v>44630.75</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="2">
+        <v>44594.708333333336</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="2">
+        <v>44594.670138888891</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2">
+        <v>44494.708333333336</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="2">
+        <v>44494.670138888891</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="2">
+        <v>44405.708333333336</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="2">
+        <v>44405.670138888891</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="2">
+        <v>44342.541666666664</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="2">
+        <v>44314.708333333336</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="2">
+        <v>44314.670138888891</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="4">
+        <v>44297</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2">
+        <v>44257.583333333336</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="2">
+        <v>44223.708333333336</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="2">
+        <v>44223.670138888891</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="2">
+        <v>44133.75</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="2">
+        <v>44133.670138888891</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="4">
+        <v>44123</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="4">
+        <v>44111</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="2">
+        <v>44042.75</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="2">
+        <v>44042.670138888891</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="2">
+        <v>43978.541666666664</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="2">
+        <v>43950.708333333336</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="2">
+        <v>43950.670138888891</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="2">
+        <v>43859.708333333336</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2">
+        <v>43859.670138888891</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2">
+        <v>43782.434027777781</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="2">
+        <v>43782.40625</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="4">
+        <v>43775</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="2">
+        <v>43768.708333333336</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="2">
+        <v>43768.670138888891</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="4">
+        <v>43760</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="4">
+        <v>43745</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="4">
+        <v>43723</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="2">
+        <v>43670.708333333336</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="2">
+        <v>43670.670138888891</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="4">
+        <v>43635</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="4">
+        <v>43627</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="4">
+        <v>43626</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="4">
+        <v>43620</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="2">
+        <v>43615.583333333336</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="4">
+        <v>43591</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="2">
+        <v>43579.708333333336</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="2">
+        <v>43579.670138888891</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="4">
+        <v>43528</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="4">
+        <v>43528</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="2">
+        <v>43522.625</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="4">
+        <v>43520</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="2">
+        <v>43495.708333333336</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="2">
+        <v>43495.670138888891</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="4">
+        <v>43432</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="2">
+        <v>43403.708333333336</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="2">
+        <v>43403.670138888891</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="4">
+        <v>43395</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="4">
+        <v>43394</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="2">
+        <v>43306.708333333336</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="2">
+        <v>43306.670138888891</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="4">
+        <v>43254</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="2">
+        <v>43251.583333333336</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="2">
+        <v>43215.708333333336</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="2">
+        <v>43215.670138888891</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="2">
+        <v>43159.625</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="2">
+        <v>43131.708333333336</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="2">
+        <v>43131.670138888891</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="2">
+        <v>43074.604166666664</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="2">
+        <v>43040.708333333336</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="2">
+        <v>43040.670138888891</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="2">
+        <v>42942.708333333336</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="2">
+        <v>42942.670138888891</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="4">
+        <v>42886</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="2">
+        <v>42858.708333333336</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="2">
+        <v>42858.674305555556</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="2">
+        <v>42767.708333333336</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="2">
+        <v>42767.667361111111</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="2">
+        <v>42676.708333333336</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="2">
+        <v>42676.670138888891</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="4">
+        <v>42667</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="2">
+        <v>42578.708333333336</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A116" s="2">
+        <v>42578.670138888891</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="2">
+        <v>42541.583333333336</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A118" s="2">
+        <v>42487.708333333336</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="4">
+        <v>42486</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="2">
+        <v>42431.625</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="2">
+        <v>42423.597222222219</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="2">
+        <v>42409.708333333336</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A123" s="2">
+        <v>42396.708333333336</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A124" s="4">
+        <v>42395</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A125" s="2">
+        <v>42346.385416666664</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A126" s="2">
+        <v>42312.708333333336</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A127" s="4">
+        <v>42311</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A128" s="2">
+        <v>42304.694444444445</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A129" s="2">
+        <v>42303.590277777781</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A130" s="2">
+        <v>42214.708333333336</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A131" s="4">
+        <v>42213</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A132" s="2">
+        <v>42166.583333333336</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A133" s="2">
+        <v>42142.444444444445</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A134" s="2">
+        <v>42116.708333333336</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A135" s="4">
+        <v>42115</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A136" s="2">
+        <v>42065.552083333336</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A137" s="2">
+        <v>42046.555555555555</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A138" s="2">
+        <v>42032.708333333336</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A139" s="4">
+        <v>42031</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A140" s="4"/>
+      <c r="B140" s="3"/>
+    </row>
+    <row r="141" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A141" s="4"/>
+      <c r="B141" s="3"/>
+    </row>
+    <row r="142" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A142" s="2"/>
+      <c r="B142" s="3"/>
+    </row>
+    <row r="143" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A143" s="2"/>
+      <c r="B143" s="3"/>
+    </row>
+    <row r="144" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A144" s="2"/>
+      <c r="B144" s="3"/>
+    </row>
+    <row r="145" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A145" s="4"/>
+      <c r="B145" s="3"/>
+    </row>
+    <row r="146" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A146" s="2"/>
+      <c r="B146" s="3"/>
+    </row>
+    <row r="147" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A147" s="2"/>
+      <c r="B147" s="3"/>
+    </row>
+    <row r="148" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A148" s="2"/>
+      <c r="B148" s="3"/>
+    </row>
+    <row r="149" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A149" s="4"/>
+      <c r="B149" s="3"/>
+    </row>
+    <row r="150" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A150" s="2"/>
+      <c r="B150" s="3"/>
+    </row>
+    <row r="151" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A151" s="2"/>
+      <c r="B151" s="3"/>
+    </row>
+    <row r="152" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A152" s="4"/>
+      <c r="B152" s="3"/>
+    </row>
+    <row r="153" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A153" s="2"/>
+      <c r="B153" s="3"/>
+    </row>
+    <row r="154" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A154" s="2"/>
+      <c r="B154" s="3"/>
+    </row>
+    <row r="155" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A155" s="2"/>
+      <c r="B155" s="3"/>
+    </row>
+    <row r="156" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A156" s="2"/>
+      <c r="B156" s="3"/>
+    </row>
+    <row r="157" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A157" s="4"/>
+      <c r="B157" s="3"/>
+    </row>
+    <row r="158" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A158" s="2"/>
+      <c r="B158" s="3"/>
+    </row>
+    <row r="159" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A159" s="2"/>
+      <c r="B159" s="3"/>
+    </row>
+    <row r="160" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A160" s="2"/>
+      <c r="B160" s="3"/>
+    </row>
+    <row r="161" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A161" s="2"/>
+      <c r="B161" s="3"/>
+    </row>
+    <row r="162" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A162" s="2"/>
+      <c r="B162" s="3"/>
+    </row>
+    <row r="163" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A163" s="2"/>
+      <c r="B163" s="3"/>
+    </row>
+    <row r="164" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A164" s="2"/>
+      <c r="B164" s="3"/>
+    </row>
+    <row r="165" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A165" s="2"/>
+      <c r="B165" s="3"/>
+    </row>
+    <row r="166" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A166" s="2"/>
+      <c r="B166" s="3"/>
+    </row>
+    <row r="167" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A167" s="2"/>
+      <c r="B167" s="3"/>
+    </row>
+    <row r="168" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A168" s="2"/>
+      <c r="B168" s="3"/>
+    </row>
+    <row r="169" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A169" s="2"/>
+      <c r="B169" s="3"/>
+    </row>
+    <row r="170" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A170" s="2"/>
+      <c r="B170" s="3"/>
+    </row>
+    <row r="171" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A171" s="2"/>
+      <c r="B171" s="3"/>
+    </row>
+    <row r="172" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A172" s="2"/>
+      <c r="B172" s="3"/>
+    </row>
+    <row r="173" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A173" s="2"/>
+      <c r="B173" s="3"/>
+    </row>
+    <row r="174" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A174" s="2"/>
+      <c r="B174" s="3"/>
+    </row>
+    <row r="175" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A175" s="2"/>
+      <c r="B175" s="3"/>
+    </row>
+    <row r="176" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A176" s="2"/>
+      <c r="B176" s="3"/>
+    </row>
+    <row r="177" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A177" s="2"/>
+      <c r="B177" s="3"/>
+    </row>
+    <row r="178" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A178" s="2"/>
+      <c r="B178" s="3"/>
+    </row>
+    <row r="179" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A179" s="2"/>
+      <c r="B179" s="3"/>
+    </row>
+    <row r="180" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A180" s="2"/>
+      <c r="B180" s="3"/>
+    </row>
+    <row r="181" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A181" s="2"/>
+      <c r="B181" s="3"/>
+    </row>
+    <row r="182" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A182" s="2"/>
+      <c r="B182" s="3"/>
+    </row>
+    <row r="183" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A183" s="2"/>
+      <c r="B183" s="3"/>
+    </row>
+    <row r="184" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A184" s="2"/>
+      <c r="B184" s="3"/>
+    </row>
+    <row r="185" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A185" s="2"/>
+      <c r="B185" s="3"/>
+    </row>
+    <row r="186" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A186" s="2"/>
+      <c r="B186" s="3"/>
+    </row>
+    <row r="187" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A187" s="4"/>
+      <c r="B187" s="3"/>
+    </row>
+    <row r="188" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A188" s="2"/>
+      <c r="B188" s="3"/>
+    </row>
+    <row r="189" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A189" s="2"/>
+      <c r="B189" s="3"/>
+    </row>
+    <row r="190" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A190" s="2"/>
+      <c r="B190" s="3"/>
+    </row>
+    <row r="191" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A191" s="2"/>
+      <c r="B191" s="3"/>
+    </row>
+    <row r="192" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A192" s="2"/>
+      <c r="B192" s="3"/>
+    </row>
+    <row r="193" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A193" s="4"/>
+      <c r="B193" s="3"/>
+    </row>
+    <row r="194" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A194" s="4"/>
+      <c r="B194" s="3"/>
+    </row>
+    <row r="195" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A195" s="2"/>
+      <c r="B195" s="3"/>
+    </row>
+    <row r="196" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A196" s="2"/>
+      <c r="B196" s="3"/>
+    </row>
+    <row r="197" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A197" s="2"/>
+      <c r="B197" s="3"/>
+    </row>
+    <row r="198" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A198" s="2"/>
+      <c r="B198" s="3"/>
+    </row>
+    <row r="199" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A199" s="2"/>
+      <c r="B199" s="3"/>
+    </row>
+    <row r="200" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A200" s="2"/>
+      <c r="B200" s="3"/>
+    </row>
+    <row r="201" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A201" s="2"/>
+      <c r="B201" s="3"/>
+    </row>
+    <row r="202" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A202" s="2"/>
+      <c r="B202" s="3"/>
+    </row>
+    <row r="203" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A203" s="2"/>
+      <c r="B203" s="3"/>
+    </row>
+    <row r="204" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A204" s="4"/>
+      <c r="B204" s="3"/>
+    </row>
+    <row r="205" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A205" s="2"/>
+      <c r="B205" s="3"/>
+    </row>
+    <row r="206" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A206" s="2"/>
+      <c r="B206" s="3"/>
+    </row>
+    <row r="207" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A207" s="4"/>
+      <c r="B207" s="3"/>
+    </row>
+    <row r="208" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A208" s="4"/>
+      <c r="B208" s="3"/>
+    </row>
+    <row r="209" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A209" s="4"/>
+      <c r="B209" s="3"/>
+    </row>
+    <row r="210" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A210" s="2"/>
+      <c r="B210" s="3"/>
+    </row>
+    <row r="211" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A211" s="2"/>
+      <c r="B211" s="3"/>
+    </row>
+    <row r="212" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A212" s="4"/>
+      <c r="B212" s="3"/>
+    </row>
+    <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A213" s="4"/>
+      <c r="B213" s="3"/>
+    </row>
+    <row r="214" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A214" s="4"/>
+      <c r="B214" s="3"/>
+    </row>
+    <row r="215" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A215" s="4"/>
+      <c r="B215" s="3"/>
+    </row>
+    <row r="216" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A216" s="2"/>
+      <c r="B216" s="3"/>
+    </row>
+    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A217" s="4"/>
+      <c r="B217" s="3"/>
+    </row>
+    <row r="218" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A218" s="2"/>
+      <c r="B218" s="3"/>
+    </row>
+    <row r="219" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A219" s="2"/>
+      <c r="B219" s="3"/>
+    </row>
+    <row r="220" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A220" s="4"/>
+      <c r="B220" s="3"/>
+    </row>
+    <row r="221" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A221" s="4"/>
+      <c r="B221" s="3"/>
+    </row>
+    <row r="222" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A222" s="2"/>
+      <c r="B222" s="3"/>
+    </row>
+    <row r="223" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A223" s="4"/>
+      <c r="B223" s="3"/>
+    </row>
+    <row r="224" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A224" s="2"/>
+      <c r="B224" s="3"/>
+    </row>
+    <row r="225" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A225" s="2"/>
+      <c r="B225" s="3"/>
+    </row>
+    <row r="226" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A226" s="4"/>
+      <c r="B226" s="3"/>
+    </row>
+    <row r="227" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A227" s="2"/>
+      <c r="B227" s="3"/>
+    </row>
+    <row r="228" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A228" s="2"/>
+      <c r="B228" s="3"/>
+    </row>
+    <row r="229" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A229" s="4"/>
+      <c r="B229" s="3"/>
+    </row>
+    <row r="230" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A230" s="4"/>
+      <c r="B230" s="3"/>
+    </row>
+    <row r="231" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A231" s="2"/>
+      <c r="B231" s="3"/>
+    </row>
+    <row r="232" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A232" s="2"/>
+      <c r="B232" s="3"/>
+    </row>
+    <row r="233" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A233" s="4"/>
+      <c r="B233" s="3"/>
+    </row>
+    <row r="234" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A234" s="2"/>
+      <c r="B234" s="3"/>
+    </row>
+    <row r="235" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A235" s="2"/>
+      <c r="B235" s="3"/>
+    </row>
+    <row r="236" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A236" s="2"/>
+      <c r="B236" s="3"/>
+    </row>
+    <row r="237" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A237" s="2"/>
+      <c r="B237" s="3"/>
+    </row>
+    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A238" s="2"/>
+      <c r="B238" s="3"/>
+    </row>
+    <row r="239" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A239" s="2"/>
+      <c r="B239" s="3"/>
+    </row>
+    <row r="240" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A240" s="2"/>
+      <c r="B240" s="3"/>
+    </row>
+    <row r="241" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A241" s="2"/>
+      <c r="B241" s="3"/>
+    </row>
+    <row r="242" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A242" s="2"/>
+      <c r="B242" s="3"/>
+    </row>
+    <row r="243" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A243" s="2"/>
+      <c r="B243" s="3"/>
+    </row>
+    <row r="244" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A244" s="2"/>
+      <c r="B244" s="3"/>
+    </row>
+    <row r="245" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A245" s="4"/>
+      <c r="B245" s="3"/>
+    </row>
+    <row r="246" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A246" s="2"/>
+      <c r="B246" s="3"/>
+    </row>
+    <row r="247" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A247" s="2"/>
+      <c r="B247" s="3"/>
+    </row>
+    <row r="248" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A248" s="2"/>
+      <c r="B248" s="3"/>
+    </row>
+    <row r="249" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A249" s="2"/>
+      <c r="B249" s="3"/>
+    </row>
+    <row r="250" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A250" s="2"/>
+      <c r="B250" s="3"/>
+    </row>
+    <row r="251" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A251" s="2"/>
+      <c r="B251" s="3"/>
+    </row>
+    <row r="252" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A252" s="4"/>
+      <c r="B252" s="3"/>
+    </row>
+    <row r="253" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A253" s="2"/>
+      <c r="B253" s="3"/>
+    </row>
+    <row r="254" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A254" s="2"/>
+      <c r="B254" s="3"/>
+    </row>
+    <row r="255" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A255" s="2"/>
+      <c r="B255" s="3"/>
+    </row>
+    <row r="256" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A256" s="2"/>
+      <c r="B256" s="3"/>
+    </row>
+    <row r="257" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A257" s="4"/>
+      <c r="B257" s="3"/>
+    </row>
+    <row r="258" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A258" s="2"/>
+      <c r="B258" s="3"/>
+    </row>
+    <row r="259" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A259" s="2"/>
+      <c r="B259" s="3"/>
+    </row>
+    <row r="260" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A260" s="2"/>
+      <c r="B260" s="3"/>
+    </row>
+    <row r="261" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A261" s="2"/>
+      <c r="B261" s="3"/>
+    </row>
+    <row r="262" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A262" s="4"/>
+      <c r="B262" s="3"/>
+    </row>
+    <row r="263" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A263" s="2"/>
+      <c r="B263" s="3"/>
+    </row>
+    <row r="264" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A264" s="2"/>
+      <c r="B264" s="3"/>
+    </row>
+    <row r="265" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A265" s="4"/>
+      <c r="B265" s="3"/>
+    </row>
+    <row r="266" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A266" s="2"/>
+      <c r="B266" s="3"/>
+    </row>
+    <row r="267" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A267" s="2"/>
+      <c r="B267" s="3"/>
+    </row>
+    <row r="268" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A268" s="2"/>
+      <c r="B268" s="3"/>
+    </row>
+    <row r="269" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A269" s="4"/>
+      <c r="B269" s="3"/>
+    </row>
+    <row r="270" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A270" s="2"/>
+      <c r="B270" s="3"/>
+    </row>
+    <row r="271" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A271" s="2"/>
+      <c r="B271" s="3"/>
+    </row>
+    <row r="272" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A272" s="2"/>
+      <c r="B272" s="3"/>
+    </row>
+    <row r="273" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A273" s="4"/>
+      <c r="B273" s="3"/>
+    </row>
+    <row r="274" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A274" s="2"/>
+      <c r="B274" s="3"/>
+    </row>
+    <row r="275" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A275" s="2"/>
+      <c r="B275" s="3"/>
+    </row>
+    <row r="276" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A276" s="2"/>
+      <c r="B276" s="3"/>
+    </row>
+    <row r="277" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A277" s="4"/>
+      <c r="B277" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>